<commit_message>
新增 CalculationEngine.unitypackage 並增加FormulaScene跟CharacterFormula ScriptableObject
</commit_message>
<xml_diff>
--- a/Assets/GameData/Excel/Character.xlsx
+++ b/Assets/GameData/Excel/Character.xlsx
@@ -1,98 +1,450 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowWidth="19095" windowHeight="9975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CharacterCC" sheetId="1" r:id="rId1"/>
+    <sheet name="CharacterFormula" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
   <si>
     <t>LV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AGI</t>
   </si>
   <si>
     <t>STR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DEX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>NAME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AGI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_Have_Bug</t>
+  </si>
+  <si>
+    <t>JOHN CENA</t>
   </si>
   <si>
     <t>star</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>sss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>sdew</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>kgflj</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JOHN CENA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>我是後來新增的傢伙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT_Have_Bug</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stat</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>MIN((5*(SkillLevel*0.6)),2)+10</t>
+  </si>
+  <si>
+    <t>5*(SkillLevel*0.2)+10</t>
+  </si>
+  <si>
+    <t>ITL</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>5*((STR*0.5)+(DEX*0.39)+(ITL*0.23))</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>5*((STR*0.01)+(DEX*0.12)+(ITL*0.87))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="新細明體"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="新細明體"/>
-      <family val="3"/>
-      <charset val="136"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="新細明體"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="新細明體"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -100,26 +452,309 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
+    <cellStyle name="20% - 輔色2" xfId="2" builtinId="34"/>
+    <cellStyle name="千分位[0]" xfId="3" builtinId="6"/>
+    <cellStyle name="千分位" xfId="4" builtinId="3"/>
+    <cellStyle name="20% - 輔色1" xfId="5" builtinId="30"/>
+    <cellStyle name="貨幣" xfId="6" builtinId="4"/>
+    <cellStyle name="備註" xfId="7" builtinId="10"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="8" builtinId="9"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="20% - 輔色5" xfId="10" builtinId="46"/>
+    <cellStyle name="40% - 輔色3" xfId="11" builtinId="39"/>
+    <cellStyle name="60% - 輔色1" xfId="12" builtinId="32"/>
+    <cellStyle name="貨幣[0]" xfId="13" builtinId="7"/>
+    <cellStyle name="警告文字" xfId="14" builtinId="11"/>
+    <cellStyle name="標題" xfId="15" builtinId="15"/>
+    <cellStyle name="說明文字" xfId="16" builtinId="53"/>
+    <cellStyle name="40% - 輔色6" xfId="17" builtinId="51"/>
+    <cellStyle name="60% - 輔色4" xfId="18" builtinId="44"/>
+    <cellStyle name="標題 1" xfId="19" builtinId="16"/>
+    <cellStyle name="60% - 輔色5" xfId="20" builtinId="48"/>
+    <cellStyle name="標題 2" xfId="21" builtinId="17"/>
+    <cellStyle name="60% - 輔色6" xfId="22" builtinId="52"/>
+    <cellStyle name="標題 3" xfId="23" builtinId="18"/>
+    <cellStyle name="標題 4" xfId="24" builtinId="19"/>
+    <cellStyle name="好" xfId="25" builtinId="26"/>
+    <cellStyle name="輸入" xfId="26" builtinId="20"/>
+    <cellStyle name="輸出" xfId="27" builtinId="21"/>
+    <cellStyle name="計算方式" xfId="28" builtinId="22"/>
+    <cellStyle name="檢查儲存格" xfId="29" builtinId="23"/>
+    <cellStyle name="連結的儲存格" xfId="30" builtinId="24"/>
+    <cellStyle name="加總" xfId="31" builtinId="25"/>
+    <cellStyle name="壞" xfId="32" builtinId="27"/>
+    <cellStyle name="中性" xfId="33" builtinId="28"/>
+    <cellStyle name="輔色1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 輔色3" xfId="35" builtinId="38"/>
+    <cellStyle name="40% - 輔色1" xfId="36" builtinId="31"/>
+    <cellStyle name="輔色2" xfId="37" builtinId="33"/>
+    <cellStyle name="20% - 輔色4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 輔色2" xfId="39" builtinId="35"/>
+    <cellStyle name="20% - 輔色6" xfId="40" builtinId="50"/>
+    <cellStyle name="40% - 輔色4" xfId="41" builtinId="43"/>
+    <cellStyle name="60% - 輔色2" xfId="42" builtinId="36"/>
+    <cellStyle name="輔色3" xfId="43" builtinId="37"/>
+    <cellStyle name="40% - 輔色5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 輔色3" xfId="45" builtinId="40"/>
+    <cellStyle name="輔色4" xfId="46" builtinId="41"/>
+    <cellStyle name="輔色5" xfId="47" builtinId="45"/>
+    <cellStyle name="輔色6" xfId="48" builtinId="49"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -166,7 +801,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,7 +836,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -409,40 +1044,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
-    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>100</v>
       </c>
@@ -456,13 +1092,13 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>5</v>
       </c>
@@ -476,13 +1112,13 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1</v>
       </c>
@@ -496,13 +1132,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1122</v>
       </c>
@@ -516,13 +1152,13 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>3</v>
       </c>
@@ -536,13 +1172,13 @@
         <v>3000</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>999</v>
       </c>
@@ -556,15 +1192,83 @@
         <v>6666</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelRow="5" outlineLevelCol="1"/>
+  <cols>
+    <col min="2" max="2" width="36.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>